<commit_message>
plotting pacing rate for each job+host type
</commit_message>
<xml_diff>
--- a/src/data/statistics (pacing).xlsx
+++ b/src/data/statistics (pacing).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eashan22/Desktop/Internship 2021/bbrv2/kibana-data-retrieval/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5A6B2B-FD05-4645-893E-503334DF34E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132A862D-D3DC-2241-93CD-C6E17D086B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5680,7 +5680,7 @@
   <dimension ref="A1:AG75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5689,7 +5689,11 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="11.1640625" bestFit="1" customWidth="1"/>

</xml_diff>